<commit_message>
Inner Transition Surface modified
</commit_message>
<xml_diff>
--- a/CSAY Obstacle Height Calculation/Datagridviews.xlsx
+++ b/CSAY Obstacle Height Calculation/Datagridviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VBStudio\CSAY_OHC\CSAY Obstacle Height Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC9940-35D2-45B2-887D-C54FDAF20C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E66C5-945F-41D6-8D02-B49FC841F5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="190">
   <si>
     <t>A</t>
   </si>
@@ -525,12 +525,6 @@
   </si>
   <si>
     <t>T_D</t>
-  </si>
-  <si>
-    <t>del_x</t>
-  </si>
-  <si>
-    <t>del_y</t>
   </si>
   <si>
     <t>Trans_AB</t>
@@ -618,7 +612,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +631,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -650,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -660,6 +660,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O66" sqref="O66"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,48 +1758,48 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="10">
         <v>27.505703209903501</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="10">
         <v>83.407881265866806</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="10">
         <v>441517.29905657098</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="10">
         <v>3042588.1111251302</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="10">
         <v>27.504632456245002</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="10">
         <v>83.407696840714294</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="10">
         <v>441498.516998337</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="10">
         <v>3042469.59004361</v>
       </c>
     </row>
@@ -2338,25 +2356,25 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="6">
         <v>27.501894794133499</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="6">
         <v>83.435495738310493</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="6">
         <v>444242.87281514402</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="6">
         <v>3042153.5371425799</v>
       </c>
     </row>
@@ -2384,98 +2402,98 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="9">
         <v>62</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="10">
         <v>27.507439043980899</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="10">
         <v>83.395280998306504</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63" s="10">
         <v>440273.69996239402</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="10">
         <v>3042786.39418591</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="9">
         <v>63</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="10">
         <v>27.506367981575</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="10">
         <v>83.395098860831993</v>
       </c>
-      <c r="F64" s="3">
+      <c r="F64" s="10">
         <v>440255.13187117199</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G64" s="10">
         <v>3042667.8394699199</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
         <v>64</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="10">
         <v>27.508678910576801</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="10">
         <v>83.386275594224301</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="10">
         <v>439384.92294447799</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="10">
         <v>3042928.10359145</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
         <v>65</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="10">
         <v>27.507607837287999</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="10">
         <v>83.386093542288506</v>
       </c>
-      <c r="F66" s="3">
+      <c r="F66" s="10">
         <v>439366.35484167899</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="10">
         <v>3042809.5488015399</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2497,29 +2515,8 @@
       <c r="G67" s="3">
         <v>3042353.3282239698</v>
       </c>
-      <c r="K67" t="s">
-        <v>147</v>
-      </c>
-      <c r="L67" t="s">
-        <v>148</v>
-      </c>
-      <c r="M67" t="s">
-        <v>149</v>
-      </c>
-      <c r="N67" t="s">
-        <v>150</v>
-      </c>
-      <c r="O67" t="s">
-        <v>166</v>
-      </c>
-      <c r="P67" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2541,36 +2538,8 @@
       <c r="G68" s="3">
         <v>3041410.09837018</v>
       </c>
-      <c r="K68">
-        <f>F67</f>
-        <v>445641.37977928598</v>
-      </c>
-      <c r="L68">
-        <f>G67</f>
-        <v>3042353.3282239698</v>
-      </c>
-      <c r="M68">
-        <f>F68</f>
-        <v>445491.905965738</v>
-      </c>
-      <c r="N68">
-        <f>G68</f>
-        <v>3041410.09837018</v>
-      </c>
-      <c r="O68">
-        <f>M68-K68</f>
-        <v>-149.47381354798563</v>
-      </c>
-      <c r="P68">
-        <f>N68-L68</f>
-        <v>-943.22985378978774</v>
-      </c>
-      <c r="Q68">
-        <f>SQRT(O68*O68+P68*P68)</f>
-        <v>954.99998849051428</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -2593,7 +2562,7 @@
         <v>3043553.1393051301</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -2616,7 +2585,7 @@
         <v>3042609.6411935999</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2624,6 +2593,37 @@
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2634,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0228FA5-250D-4082-9F1E-2E5C8C9FD3FC}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B52" sqref="B52:E57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,11 +2982,11 @@
         <v>3182417.3367330302</v>
       </c>
       <c r="Q11">
-        <f>M11-O11</f>
+        <f t="shared" ref="Q11:R13" si="0">M11-O11</f>
         <v>3.524958103184872E-13</v>
       </c>
       <c r="R11">
-        <f>N11-P11</f>
+        <f t="shared" si="0"/>
         <v>-1.4714896678924561E-7</v>
       </c>
     </row>
@@ -3042,11 +3042,11 @@
         <v>3182631.97115209</v>
       </c>
       <c r="Q12">
-        <f>M12-O12</f>
+        <f t="shared" si="0"/>
         <v>-1.0680345496894006E-13</v>
       </c>
       <c r="R12">
-        <f>N12-P12</f>
+        <f t="shared" si="0"/>
         <v>4.4703483581542969E-8</v>
       </c>
     </row>
@@ -3102,11 +3102,11 @@
         <v>3182417.3367330302</v>
       </c>
       <c r="Q13" s="4">
-        <f>M13-O13</f>
+        <f t="shared" si="0"/>
         <v>2.4729662762013049E-12</v>
       </c>
       <c r="R13" s="4">
-        <f>N13-P13</f>
+        <f t="shared" si="0"/>
         <v>-1.0807998478412628E-6</v>
       </c>
     </row>
@@ -3552,19 +3552,19 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="8">
         <v>6.3103351108138899</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="8">
         <v>256465.996856735</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="8">
         <v>120.000051992599</v>
       </c>
     </row>
@@ -3790,36 +3790,36 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="7">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="8">
         <v>6.3848628582221902</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="8">
         <v>231699.19984395601</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="8">
         <v>119.999977899119</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="7">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="8">
         <v>6.3848628582221902</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="8">
         <v>237515.62862043301</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="8">
         <v>120.000052719321</v>
       </c>
     </row>
@@ -3896,7 +3896,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C52" s="3">
         <v>6.3103351108138899</v>
@@ -3913,7 +3913,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C53" s="3">
         <v>6.3848628582221902</v>
@@ -4009,8 +4009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4CD569-0378-402B-A18B-15DA6B16D28E}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4026,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D1" s="3"/>
     </row>
@@ -4036,7 +4036,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D2" s="3">
         <v>5</v>
@@ -4048,7 +4048,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D3" s="3">
         <v>100</v>
@@ -4060,7 +4060,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -4070,7 +4070,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D5" s="3">
         <v>45</v>
@@ -4082,7 +4082,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D6" s="3">
         <v>4000</v>
@@ -4094,7 +4094,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -4104,7 +4104,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D8" s="3">
         <v>120</v>
@@ -4119,7 +4119,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D9" s="3">
         <v>60</v>
@@ -4131,7 +4131,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D10" s="3">
         <v>900</v>
@@ -4143,7 +4143,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
@@ -4155,7 +4155,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -4165,7 +4165,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D13" s="3">
         <v>280</v>
@@ -4177,7 +4177,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D14" s="3">
         <v>60</v>
@@ -4189,7 +4189,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D15" s="3">
         <v>15</v>
@@ -4201,7 +4201,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -4211,7 +4211,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D17" s="3">
         <v>3000</v>
@@ -4223,7 +4223,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -4235,7 +4235,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -4245,7 +4245,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D20" s="3">
         <v>3600</v>
@@ -4257,7 +4257,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D21" s="3">
         <v>2.5</v>
@@ -4269,7 +4269,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D22" s="3"/>
     </row>
@@ -4279,7 +4279,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D23" s="3">
         <v>8400</v>
@@ -4291,7 +4291,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D24" s="3">
         <v>15000</v>
@@ -4303,7 +4303,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -4313,7 +4313,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D26" s="3">
         <v>14.3</v>
@@ -4325,7 +4325,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D27" s="3"/>
     </row>
@@ -4335,7 +4335,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D28" s="3">
         <v>33.299999999999997</v>
@@ -4347,7 +4347,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -4357,7 +4357,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D30" s="3">
         <v>120</v>
@@ -4369,7 +4369,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D31" s="3">
         <v>1800</v>
@@ -4381,7 +4381,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D32" s="3">
         <v>10</v>
@@ -4393,7 +4393,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D33" s="3">
         <v>3.33</v>
@@ -4405,7 +4405,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -4415,7 +4415,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D35" s="3">
         <v>180</v>
@@ -4427,7 +4427,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D36" s="3">
         <v>60</v>
@@ -4439,7 +4439,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D37" s="3">
         <v>12.5</v>
@@ -4451,7 +4451,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D38" s="3">
         <v>1800</v>
@@ -4463,7 +4463,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D39" s="3">
         <v>15000</v>
@@ -4475,7 +4475,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D40" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
IHS withing strip removed and extract coord by click added
</commit_message>
<xml_diff>
--- a/CSAY Obstacle Height Calculation/Datagridviews.xlsx
+++ b/CSAY Obstacle Height Calculation/Datagridviews.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VBStudio\CSAY_OHC\CSAY Obstacle Height Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E66C5-945F-41D6-8D02-B49FC841F5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC93E52-889F-4DE9-B1C9-72E6E8F043B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,12 +631,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -650,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -664,12 +658,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1758,48 +1746,48 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="3">
         <v>27.505703209903501</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="3">
         <v>83.407881265866806</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="3">
         <v>441517.29905657098</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="3">
         <v>3042588.1111251302</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="3">
         <v>27.504632456245002</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="3">
         <v>83.407696840714294</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="3">
         <v>441498.516998337</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="3">
         <v>3042469.59004361</v>
       </c>
     </row>
@@ -2402,94 +2390,94 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+      <c r="A63" s="2">
         <v>62</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="3">
         <v>27.507439043980899</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63" s="3">
         <v>83.395280998306504</v>
       </c>
-      <c r="F63" s="10">
+      <c r="F63" s="3">
         <v>440273.69996239402</v>
       </c>
-      <c r="G63" s="10">
+      <c r="G63" s="3">
         <v>3042786.39418591</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+      <c r="A64" s="2">
         <v>63</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="3">
         <v>27.506367981575</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="3">
         <v>83.395098860831993</v>
       </c>
-      <c r="F64" s="10">
+      <c r="F64" s="3">
         <v>440255.13187117199</v>
       </c>
-      <c r="G64" s="10">
+      <c r="G64" s="3">
         <v>3042667.8394699199</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+      <c r="A65" s="2">
         <v>64</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="3">
         <v>27.508678910576801</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="3">
         <v>83.386275594224301</v>
       </c>
-      <c r="F65" s="10">
+      <c r="F65" s="3">
         <v>439384.92294447799</v>
       </c>
-      <c r="G65" s="10">
+      <c r="G65" s="3">
         <v>3042928.10359145</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="3">
         <v>27.507607837287999</v>
       </c>
-      <c r="E66" s="10">
+      <c r="E66" s="3">
         <v>83.386093542288506</v>
       </c>
-      <c r="F66" s="10">
+      <c r="F66" s="3">
         <v>439366.35484167899</v>
       </c>
-      <c r="G66" s="10">
+      <c r="G66" s="3">
         <v>3042809.5488015399</v>
       </c>
     </row>
@@ -2634,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0228FA5-250D-4082-9F1E-2E5C8C9FD3FC}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,19 +2747,19 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>6.3103351108138899</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>244582.31009977299</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>279.99998643311699</v>
       </c>
       <c r="I6" s="2">
@@ -2890,19 +2878,19 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>6.3848628582221902</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>231699.19984395601</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>279.99998762194298</v>
       </c>
       <c r="I10" t="s">
@@ -3722,36 +3710,36 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="5">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="6">
         <v>-0.15944295171089901</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="6">
         <v>3113065.9426666098</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="6">
         <v>3119.45253487641</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="6">
         <v>-0.15944325891934799</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="6">
         <v>3112782.5422495999</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="6">
         <v>3118.9471487857199</v>
       </c>
     </row>
@@ -4009,8 +3997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4CD569-0378-402B-A18B-15DA6B16D28E}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B10:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Multiple OLS data calc added
</commit_message>
<xml_diff>
--- a/CSAY Obstacle Height Calculation/Datagridviews.xlsx
+++ b/CSAY Obstacle Height Calculation/Datagridviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VBStudio\CSAY_OHC\CSAY Obstacle Height Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6776997-7B96-4905-90DD-BBA94114799C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D79F8E-A1F7-4B16-85E4-4CDC164B5B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Sheet4 (2)" sheetId="7" r:id="rId7"/>
     <sheet name="DGV10" sheetId="8" r:id="rId8"/>
     <sheet name="DGV11" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="239">
   <si>
     <t>A</t>
   </si>
@@ -687,6 +688,69 @@
   </si>
   <si>
     <t>IT</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>RL of Plinth</t>
+  </si>
+  <si>
+    <t>Height above plinth</t>
+  </si>
+  <si>
+    <t>ObstacleID</t>
+  </si>
+  <si>
+    <t>ObstacleType</t>
+  </si>
+  <si>
+    <t>Input table</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Easting_X</t>
+  </si>
+  <si>
+    <t>Northing_Y</t>
+  </si>
+  <si>
+    <t>Obstacle RL</t>
+  </si>
+  <si>
+    <t>OLS RL</t>
+  </si>
+  <si>
+    <t>Intrusion into OLS</t>
+  </si>
+  <si>
+    <t>OLS</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>Hospita</t>
+  </si>
+  <si>
+    <t>Chimney</t>
+  </si>
+  <si>
+    <t>Mast</t>
   </si>
 </sst>
 </file>
@@ -722,7 +786,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -754,11 +818,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -785,6 +886,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3142,7 +3258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>
@@ -7972,6 +8088,545 @@
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7337BFDF-F899-4334-991A-587B3E3659EC}">
+  <dimension ref="B3:V19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="J3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15">
+        <v>101</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="E5" s="15">
+        <v>27.501115240525099</v>
+      </c>
+      <c r="F5" s="15">
+        <v>83.438587188720703</v>
+      </c>
+      <c r="G5" s="15">
+        <v>108</v>
+      </c>
+      <c r="H5" s="15">
+        <v>35</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="15">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15">
+        <v>102</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E6" s="15">
+        <v>27.497460844863902</v>
+      </c>
+      <c r="F6" s="15">
+        <v>83.463306427001996</v>
+      </c>
+      <c r="G6" s="15">
+        <v>107</v>
+      </c>
+      <c r="H6" s="15">
+        <v>25.32</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="15">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15">
+        <v>103</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" s="15">
+        <v>27.495481329889</v>
+      </c>
+      <c r="F7" s="15">
+        <v>83.489227294921903</v>
+      </c>
+      <c r="G7" s="15">
+        <v>102.65</v>
+      </c>
+      <c r="H7" s="15">
+        <v>46.95</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="15">
+        <v>4</v>
+      </c>
+      <c r="C8" s="15">
+        <v>104</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="15">
+        <v>27.506139836437299</v>
+      </c>
+      <c r="F8" s="15">
+        <v>83.423995971679702</v>
+      </c>
+      <c r="G8" s="15">
+        <v>106.32</v>
+      </c>
+      <c r="H8" s="15">
+        <v>43.62</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0</v>
+      </c>
+      <c r="K8" s="18">
+        <v>1</v>
+      </c>
+      <c r="L8" s="18">
+        <v>2</v>
+      </c>
+      <c r="M8" s="18">
+        <v>3</v>
+      </c>
+      <c r="N8" s="18">
+        <v>4</v>
+      </c>
+      <c r="O8" s="18">
+        <v>5</v>
+      </c>
+      <c r="P8" s="18">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>7</v>
+      </c>
+      <c r="R8" s="18">
+        <v>8</v>
+      </c>
+      <c r="S8" s="18">
+        <v>9</v>
+      </c>
+      <c r="T8" s="18">
+        <v>10</v>
+      </c>
+      <c r="U8" s="18">
+        <v>11</v>
+      </c>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="15">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
+        <v>105</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" s="15">
+        <v>27.503399176197799</v>
+      </c>
+      <c r="F9" s="15">
+        <v>83.396530151367202</v>
+      </c>
+      <c r="G9" s="15">
+        <v>118.32</v>
+      </c>
+      <c r="H9" s="15">
+        <v>24.87</v>
+      </c>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>6</v>
+      </c>
+      <c r="C10" s="15">
+        <v>106</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="E10" s="15">
+        <v>27.462281084497601</v>
+      </c>
+      <c r="F10" s="15">
+        <v>83.373184204101605</v>
+      </c>
+      <c r="G10" s="15">
+        <v>107.98</v>
+      </c>
+      <c r="H10" s="15">
+        <v>32.987000000000002</v>
+      </c>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="15">
+        <v>7</v>
+      </c>
+      <c r="C11" s="15">
+        <v>107</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="E11" s="15">
+        <v>27.5079669053416</v>
+      </c>
+      <c r="F11" s="15">
+        <v>83.388805389404297</v>
+      </c>
+      <c r="G11" s="15">
+        <v>106.35</v>
+      </c>
+      <c r="H11" s="15">
+        <v>45.65</v>
+      </c>
+      <c r="R11" t="s">
+        <v>139</v>
+      </c>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="15">
+        <v>8</v>
+      </c>
+      <c r="C12" s="15">
+        <v>108</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E12" s="15">
+        <v>27.532324924454599</v>
+      </c>
+      <c r="F12" s="15">
+        <v>83.295593261718807</v>
+      </c>
+      <c r="G12" s="15">
+        <v>109.324</v>
+      </c>
+      <c r="H12" s="15">
+        <v>62.87</v>
+      </c>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="15">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15">
+        <v>109</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="E13" s="15">
+        <v>27.546937145643199</v>
+      </c>
+      <c r="F13" s="15">
+        <v>83.2489013671875</v>
+      </c>
+      <c r="G13" s="15">
+        <v>102.35</v>
+      </c>
+      <c r="H13" s="15">
+        <v>15.65</v>
+      </c>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="15">
+        <v>10</v>
+      </c>
+      <c r="C14" s="15">
+        <v>110</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="E14" s="15">
+        <v>27.528062660603801</v>
+      </c>
+      <c r="F14" s="15">
+        <v>83.447685241699205</v>
+      </c>
+      <c r="G14" s="15">
+        <v>107.03</v>
+      </c>
+      <c r="H14" s="15">
+        <v>18.95</v>
+      </c>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="15">
+        <v>11</v>
+      </c>
+      <c r="C15" s="15">
+        <v>111</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" s="15">
+        <v>27.476598013637801</v>
+      </c>
+      <c r="F15" s="15">
+        <v>83.529739379882798</v>
+      </c>
+      <c r="G15" s="15">
+        <v>108.32</v>
+      </c>
+      <c r="H15" s="15">
+        <v>24.625</v>
+      </c>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="15">
+        <v>12</v>
+      </c>
+      <c r="C16" s="15">
+        <v>112</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="15">
+        <v>27.513143435807201</v>
+      </c>
+      <c r="F16" s="15">
+        <v>83.3477783203125</v>
+      </c>
+      <c r="G16" s="15">
+        <v>109.45</v>
+      </c>
+      <c r="H16" s="15">
+        <v>265.35000000000002</v>
+      </c>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="15">
+        <v>13</v>
+      </c>
+      <c r="C17" s="15">
+        <v>113</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="E17" s="15">
+        <v>27.509793943906701</v>
+      </c>
+      <c r="F17" s="15">
+        <v>83.376960754394503</v>
+      </c>
+      <c r="G17" s="15">
+        <v>106.04</v>
+      </c>
+      <c r="H17" s="15">
+        <v>25.35</v>
+      </c>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
+        <v>14</v>
+      </c>
+      <c r="C18" s="15">
+        <v>114</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" s="15">
+        <v>27.519842113641001</v>
+      </c>
+      <c r="F18" s="15">
+        <v>83.330268859863295</v>
+      </c>
+      <c r="G18" s="15">
+        <v>105.02500000000001</v>
+      </c>
+      <c r="H18" s="15">
+        <v>18.324999999999999</v>
+      </c>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="15">
+        <v>15</v>
+      </c>
+      <c r="C19" s="15">
+        <v>115</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="E19" s="15">
+        <v>27.500049387657299</v>
+      </c>
+      <c r="F19" s="15">
+        <v>83.453865051269503</v>
+      </c>
+      <c r="G19" s="15">
+        <v>108.36</v>
+      </c>
+      <c r="H19" s="15">
+        <v>41.35</v>
+      </c>
+      <c r="V19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RWY designation display added
</commit_message>
<xml_diff>
--- a/CSAY Obstacle Height Calculation/Datagridviews.xlsx
+++ b/CSAY Obstacle Height Calculation/Datagridviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VBStudio\CSAY_OHC\CSAY Obstacle Height Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D79F8E-A1F7-4B16-85E4-4CDC164B5B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0426AB-6034-4E77-8DF4-3FC6DB0F7352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="Sheet4 (2)" sheetId="7" r:id="rId7"/>
     <sheet name="DGV10" sheetId="8" r:id="rId8"/>
     <sheet name="DGV11" sheetId="10" r:id="rId9"/>
-    <sheet name="Sheet3" sheetId="11" r:id="rId10"/>
+    <sheet name="Multi obs" sheetId="11" r:id="rId10"/>
+    <sheet name="plotcase" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="253">
   <si>
     <t>A</t>
   </si>
@@ -751,19 +752,67 @@
   </si>
   <si>
     <t>Mast</t>
+  </si>
+  <si>
+    <t>Plotcase No.</t>
+  </si>
+  <si>
+    <t>Shortest distance of obstacle from runway</t>
+  </si>
+  <si>
+    <t>1, 3, 5, 7</t>
+  </si>
+  <si>
+    <t>distance between obstacle and RWY point D, A, B, C respectively</t>
+  </si>
+  <si>
+    <t>2, 4, 6, 8</t>
+  </si>
+  <si>
+    <t>Perpendicula distance on sides AD, AB, BC, CD respectively</t>
+  </si>
+  <si>
+    <t>Conical, Inner Horizontal, Outer Horizontal</t>
+  </si>
+  <si>
+    <t>1 to 8</t>
+  </si>
+  <si>
+    <t>Transition, Inner Transition</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 5, 6, 7</t>
+  </si>
+  <si>
+    <t>Inner Approach, Approach, Take Off Climb</t>
+  </si>
+  <si>
+    <t>1, 8, 7, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Balked Landing</t>
+  </si>
+  <si>
+    <t>1 to 8 and within RWY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -859,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -892,14 +941,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8098,8 +8148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7337BFDF-F899-4334-991A-587B3E3659EC}">
   <dimension ref="B3:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8138,22 +8188,22 @@
       <c r="B4" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>222</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -8308,7 +8358,7 @@
       <c r="C8" s="15">
         <v>104</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>236</v>
       </c>
       <c r="E8" s="15">
@@ -8323,40 +8373,40 @@
       <c r="H8" s="15">
         <v>43.62</v>
       </c>
-      <c r="J8" s="18">
-        <v>0</v>
-      </c>
-      <c r="K8" s="18">
+      <c r="J8" s="17">
+        <v>0</v>
+      </c>
+      <c r="K8" s="17">
         <v>1</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="17">
         <v>2</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>3</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="17">
         <v>4</v>
       </c>
-      <c r="O8" s="18">
+      <c r="O8" s="17">
         <v>5</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="17">
         <v>6</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="17">
         <v>7</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="17">
         <v>8</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="17">
         <v>9</v>
       </c>
-      <c r="T8" s="18">
+      <c r="T8" s="17">
         <v>10</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="17">
         <v>11</v>
       </c>
       <c r="V8" s="2"/>
@@ -8368,7 +8418,7 @@
       <c r="C9" s="15">
         <v>105</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>233</v>
       </c>
       <c r="E9" s="15">
@@ -8392,7 +8442,7 @@
       <c r="C10" s="15">
         <v>106</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>233</v>
       </c>
       <c r="E10" s="15">
@@ -8416,7 +8466,7 @@
       <c r="C11" s="15">
         <v>107</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>235</v>
       </c>
       <c r="E11" s="15">
@@ -8443,7 +8493,7 @@
       <c r="C12" s="15">
         <v>108</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>234</v>
       </c>
       <c r="E12" s="15">
@@ -8467,7 +8517,7 @@
       <c r="C13" s="15">
         <v>109</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>234</v>
       </c>
       <c r="E13" s="15">
@@ -8491,7 +8541,7 @@
       <c r="C14" s="15">
         <v>110</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>233</v>
       </c>
       <c r="E14" s="15">
@@ -8515,7 +8565,7 @@
       <c r="C15" s="15">
         <v>111</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>237</v>
       </c>
       <c r="E15" s="15">
@@ -8539,7 +8589,7 @@
       <c r="C16" s="15">
         <v>112</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>237</v>
       </c>
       <c r="E16" s="15">
@@ -8563,7 +8613,7 @@
       <c r="C17" s="15">
         <v>113</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>237</v>
       </c>
       <c r="E17" s="15">
@@ -8587,7 +8637,7 @@
       <c r="C18" s="15">
         <v>114</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>238</v>
       </c>
       <c r="E18" s="15">
@@ -8611,7 +8661,7 @@
       <c r="C19" s="15">
         <v>115</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>238</v>
       </c>
       <c r="E19" s="15">
@@ -8627,6 +8677,97 @@
         <v>41.35</v>
       </c>
       <c r="V19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382DABF1-195A-40DF-A5ED-A0FFE8A321BD}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D8" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>252</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>